<commit_message>
Gunakan Binary Search untuk menemukan awal dan akhir rentang. Meluas ke atas jika ada data dengan tanggal awal yang sama sebelum titik yang ditemukan. Meluas ke bawah jika ada data dengan tanggal akhir yang sama setelah titik yang ditemukan. Menggunakan array_slice untuk mengambil seluruh data dalam rentang yang sudah diperluas.
</commit_message>
<xml_diff>
--- a/BinarySearch/Flowers by Khansa Oktober 2024.xlsx
+++ b/BinarySearch/Flowers by Khansa Oktober 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App\Xampp\htdocs\prototype-penjualan-bunga\BinarySearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8088E93-15A9-45BD-AB01-056C347403ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6D81EF-2E0E-4525-BAB3-B7CC4E1F870A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SEPTEMBER" sheetId="1" r:id="rId1"/>
@@ -801,7 +801,7 @@
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -810,7 +810,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -3924,8 +3924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="91" workbookViewId="0">
-      <selection activeCell="I100" sqref="I100"/>
+    <sheetView topLeftCell="A24" zoomScale="74" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5998,8 +5998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="C1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -9196,8 +9196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F171"/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView zoomScale="88" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -9208,6 +9208,7 @@
     <col min="4" max="4" width="16.07421875" customWidth="1"/>
     <col min="5" max="5" width="18.15234375" customWidth="1"/>
     <col min="6" max="6" width="16.69140625" customWidth="1"/>
+    <col min="7" max="7" width="16.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -12459,6 +12460,7 @@
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12466,8 +12468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="94" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -15453,8 +15455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:B8"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="84" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A3" zoomScale="126" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -15543,7 +15545,7 @@
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -15552,7 +15554,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>

</xml_diff>